<commit_message>
feat: implement database schema and ETL pipeline
</commit_message>
<xml_diff>
--- a/backend/tests/mock_data.xlsx
+++ b/backend/tests/mock_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,98 +434,155 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>2023年采购数据</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr"/>
+      <c r="C1" t="inlineStr"/>
+      <c r="D1" t="inlineStr"/>
+      <c r="E1" t="inlineStr"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>PNs</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>Qty</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C2" s="1" t="inlineStr">
         <is>
           <t>Supp</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D2" s="1" t="inlineStr">
         <is>
           <t>Annual Spend</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E2" s="1" t="inlineStr">
         <is>
           <t>Unknown</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>A123</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>100</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Supplier A</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>X</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>B456</t>
+          <t>A123</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Supplier B</t>
+          <t>Supplier A</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>X</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>B456</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>200</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Supplier B</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>C789</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B5" t="n">
         <v>300</v>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>Supplier C</t>
         </is>
       </c>
-      <c r="D4" t="n">
+      <c r="D5" t="n">
         <v>3000</v>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>D101</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>400</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Supplier D</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>4000</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>E202</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>500</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Supplier E</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>N</t>
         </is>
       </c>
     </row>

</xml_diff>